<commit_message>
fizemos a converção das notas
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Nome</t>
   </si>
@@ -28,10 +28,16 @@
     <t>Nota Português</t>
   </si>
   <si>
-    <t>Nota Cieências</t>
-  </si>
-  <si>
-    <t>Avaliação de Matematica</t>
+    <t>Nota Ciências</t>
+  </si>
+  <si>
+    <t>Avaliação Matematica</t>
+  </si>
+  <si>
+    <t>Avaliação Português</t>
+  </si>
+  <si>
+    <t>Avaliação Ciências</t>
   </si>
   <si>
     <t>Claudio</t>
@@ -125,8 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -435,18 +444,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="69.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -468,96 +479,114 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F2" s="2">
+        <f>if C2 &lt; 7'Reprovado' else 'Aprovado'</f>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
aprendemos a pegar a quantidade de uma coluna
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Nome</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
   <si>
     <t>João</t>
@@ -131,11 +134,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -450,14 +450,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="69.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -502,18 +502,18 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2">
-        <f>if C2 &lt; 7'Reprovado' else 'Aprovado'</f>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -522,7 +522,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -530,19 +530,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -550,19 +550,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -570,19 +570,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>

</xml_diff>

<commit_message>
concluimos a primeira parte do 1 exercicio
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Nome</t>
   </si>
@@ -31,15 +31,6 @@
     <t>Nota Ciências</t>
   </si>
   <si>
-    <t>Avaliação Matematica</t>
-  </si>
-  <si>
-    <t>Avaliação Português</t>
-  </si>
-  <si>
-    <t>Avaliação Ciências</t>
-  </si>
-  <si>
     <t>Claudio</t>
   </si>
   <si>
@@ -53,9 +44,6 @@
   </si>
   <si>
     <t>9</t>
-  </si>
-  <si>
-    <t>e</t>
   </si>
   <si>
     <t>João</t>
@@ -444,7 +432,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -455,9 +443,6 @@
     <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -476,117 +461,91 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+        <v>12</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+        <v>19</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
conseguimos concluir o primeiro exercicio
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,21 @@
           <t>Nota Ciencia</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Avaliação Matematica</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Avaliação Português</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Avaliação Ciências</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +481,21 @@
       <c r="E2" t="n">
         <v>6</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Insuficiente</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Insuficiente</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Insuficiente</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -485,6 +515,21 @@
       <c r="E3" t="n">
         <v>14</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -504,6 +549,21 @@
       <c r="E4" t="n">
         <v>10</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Insuficiente</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Insuficiente</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -522,6 +582,21 @@
       </c>
       <c r="E5" t="n">
         <v>17</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criamos uma função para fazer o filtro pelo valor passado pelo usuario version 1.0
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="dados.xlsx" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dados.xlsx" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Nota Ciencia</t>
+          <t>Nota Ciências</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -466,20 +466,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>João</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>16</v>
-      </c>
-      <c r="C2" t="n">
-        <v>8</v>
-      </c>
-      <c r="D2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6</v>
+          <t>Claudio</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -500,63 +508,79 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Maria</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>17</v>
-      </c>
-      <c r="C3" t="n">
-        <v>17</v>
-      </c>
-      <c r="D3" t="n">
-        <v>19</v>
-      </c>
-      <c r="E3" t="n">
-        <v>14</v>
+          <t>João</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Suficiente</t>
+          <t>Insuficiente</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Suficiente</t>
+          <t>Insuficiente</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Suficiente</t>
+          <t>Insuficiente</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pedro</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>16</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Insuficiente</t>
+          <t>Suficiente</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Insuficiente</t>
+          <t>Suficiente</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -568,32 +592,82 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Insuficiente</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Insuficiente</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Suficiente</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Ana</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>18</v>
-      </c>
-      <c r="C5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D5" t="n">
-        <v>20</v>
-      </c>
-      <c r="E5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Suficiente</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Suficiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Suficiente</t>
         </is>

</xml_diff>